<commit_message>
with pop up window
</commit_message>
<xml_diff>
--- a/Kontakte Alle Veranstaltungen.xlsx
+++ b/Kontakte Alle Veranstaltungen.xlsx
@@ -22967,7 +22967,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A3" ySplit="2"/>
@@ -23685,7 +23685,6 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
       <c r="B19" t="inlineStr">
         <is>
           <t xml:space="preserve">ООО « СпецСтройМонтаж» 1
@@ -23703,7 +23702,6 @@
 </t>
         </is>
       </c>
-      <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
           <t>Иванюк</t>
@@ -23715,8 +23713,6 @@
 </t>
         </is>
       </c>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
           <t xml:space="preserve">+7 (911) 955-25-58
@@ -23724,6 +23720,430 @@
         </is>
       </c>
       <c r="K19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ooo-ssm@mail.ru
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AHK
+</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Координатор проекта Единое окно\nпо содействию экспорта
+</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Ботов</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Александр Ботов
+</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+7 (915) 450 08 42
+</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">botow@russland-ahk.ru
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ООО « СпецСтройМонтаж» 1
+</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ген. директор
+</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Иванюк</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Василий Валентинович Иванюк
+</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+7 (911) 955-25-58
+</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ooo-ssm@mail.ru
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AHK
+</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Координатор проекта Единое окно\nпо содействию экспорта
+</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Ботов</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Александр Ботов
+</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+7 (915) 450 08 42
+</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">botow@russland-ahk.ru
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ООО « СпецСтройМонтаж» 1
+</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ген. директор
+</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Иванюк</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Василий Валентинович Иванюк
+</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+7 (911) 955-25-58
+</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ooo-ssm@mail.ru
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AHK
+</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Координатор проекта Единое окно\nпо содействию экспорта
+</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Ботов</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Александр Ботов
+</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+7 (915) 450 08 42
+</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">botow@russland-ahk.ru
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ООО « СпецСтройМонтаж» 1
+</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ген. директор
+</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Иванюк</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Василий Валентинович Иванюк
+</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+7 (911) 955-25-58
+</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ooo-ssm@mail.ru
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AHK
+</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Координатор проекта Единое окно\nпо содействию экспорта
+</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Ботов</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Александр Ботов
+</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+7 (915) 450 08 42
+</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">botow@russland-ahk.ru
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ООО « СпецСтройМонтаж» 1
+</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ген. директор
+</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Иванюк</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Василий Валентинович Иванюк
+</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+7 (911) 955-25-58
+</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ooo-ssm@mail.ru
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AHK
+</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Москва</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Координатор проекта Единое окно\nпо содействию экспорта
+</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Ботов</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Александр Ботов
+</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+7 (915) 450 08 42
+</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">botow@russland-ahk.ru
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ООО « СпецСтройМонтаж» 1
+</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Санкт-Петербург</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ген. директор
+</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Иванюк</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Василий Валентинович Иванюк
+</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">+7 (911) 955-25-58
+</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
         <is>
           <t xml:space="preserve">ooo-ssm@mail.ru
 </t>

</xml_diff>